<commit_message>
plotted minor and major taxa amazon in nb python
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/lca/NAAF/all-stations-taxa.xlsx
+++ b/analyses/T7-incubations/unipept/lca/NAAF/all-stations-taxa.xlsx
@@ -335,8 +335,8 @@
   </sheetPr>
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O32" activeCellId="0" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>